<commit_message>
Update schedule file: Y1_B2526_Introduction_to_Histology_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y1_B2526_Introduction_to_Histology_schedule.xlsx
+++ b/modules_schedules/Y1_B2526_Introduction_to_Histology_schedule.xlsx
@@ -78,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -90,6 +90,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -457,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,30 +528,65 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>07/09/2025</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Year 1</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
           <t>B2</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>histology</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>07/09/2025</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G3" s="5" t="n">
         <v>120</v>
       </c>
     </row>

</xml_diff>